<commit_message>
een missende brouwerij toegevoegd aan dataset
</commit_message>
<xml_diff>
--- a/2019-untappd/untappd-ratings-nederlandse-bierbrouwerijen-2019.xlsx
+++ b/2019-untappd/untappd-ratings-nederlandse-bierbrouwerijen-2019.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2960" yWindow="200" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="info" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4240" uniqueCount="1691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4248" uniqueCount="1693">
   <si>
     <t>Nederlandse brouwers en brouwerijhuurders met ratings van Untappd.com</t>
   </si>
@@ -5096,6 +5096,12 @@
   </si>
   <si>
     <t>Brouwerij Emelisse</t>
+  </si>
+  <si>
+    <t>https://untappd.com/Brouwerij_Tamesteut</t>
+  </si>
+  <si>
+    <t>Brouwerij Tamesteut</t>
   </si>
 </sst>
 </file>
@@ -5539,7 +5545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -5689,11 +5695,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K526"/>
+  <dimension ref="A1:K527"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="C522" sqref="C522"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -24110,17 +24116,48 @@
         <v>1670</v>
       </c>
     </row>
+    <row r="527" spans="1:11">
+      <c r="A527">
+        <v>5</v>
+      </c>
+      <c r="B527" s="5" t="s">
+        <v>1691</v>
+      </c>
+      <c r="C527" t="s">
+        <v>1692</v>
+      </c>
+      <c r="D527" t="s">
+        <v>1692</v>
+      </c>
+      <c r="E527" t="s">
+        <v>1281</v>
+      </c>
+      <c r="F527">
+        <v>444</v>
+      </c>
+      <c r="G527" t="s">
+        <v>1360</v>
+      </c>
+      <c r="H527" t="s">
+        <v>1369</v>
+      </c>
+      <c r="I527">
+        <v>2018</v>
+      </c>
+      <c r="J527" t="s">
+        <v>1400</v>
+      </c>
+      <c r="K527" t="s">
+        <v>1669</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K526">
-    <sortState ref="A2:L526">
-      <sortCondition descending="1" ref="E1"/>
-    </sortState>
-  </autoFilter>
   <hyperlinks>
     <hyperlink ref="B104" r:id="rId1"/>
     <hyperlink ref="B298" r:id="rId2"/>
     <hyperlink ref="B491" r:id="rId3"/>
     <hyperlink ref="B18" r:id="rId4"/>
+    <hyperlink ref="B527" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>